<commit_message>
Update requests file to remove hidden sheet from view
</commit_message>
<xml_diff>
--- a/statistics_files/2024/2024.g.requests.statistics.xlsx
+++ b/statistics_files/2024/2024.g.requests.statistics.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\George\Documents\GitHub\next_statistics\statistics_files\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C61C95-AA0B-40FA-9EE9-6C2FD0CD193A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924BE8F3-9542-4D3A-93CC-ECC5FB95CC62}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11385" tabRatio="894" xr2:uid="{A4AFB16E-7F1D-4821-8B9E-72BCB5FA7E88}"/>
   </bookViews>
   <sheets>
     <sheet name="Yearly total" sheetId="1" r:id="rId1"/>
     <sheet name="January" sheetId="2" r:id="rId2"/>
-    <sheet name="JanuaryRaw" sheetId="14" r:id="rId3"/>
+    <sheet name="JanuaryRaw" sheetId="14" state="hidden" r:id="rId3"/>
     <sheet name="February" sheetId="3" r:id="rId4"/>
     <sheet name="FebruaryRaw" sheetId="15" state="hidden" r:id="rId5"/>
     <sheet name="March" sheetId="4" r:id="rId6"/>

</xml_diff>